<commit_message>
Added location data to movement
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-was-bos-041616.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-was-bos-041616.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
@@ -831,8 +831,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -948,7 +952,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -971,6 +975,10 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1238,7 +1246,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1249,8 +1257,8 @@
   <dimension ref="A1:T1399"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A691" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F691" sqref="F691"/>
+      <pane ySplit="1" topLeftCell="A1364" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1391" sqref="H1391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -36117,8 +36125,8 @@
       <c r="G823" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H823" s="9" t="s">
-        <v>20</v>
+      <c r="H823" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="I823" s="9" t="s">
         <v>20</v>
@@ -70264,7 +70272,7 @@
         <v>96</v>
       </c>
       <c r="H1365" s="15" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="I1365" s="15" t="s">
         <v>20</v>
@@ -71902,7 +71910,7 @@
         <v>110</v>
       </c>
       <c r="H1391" s="15" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="I1391" s="15" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Changed "fulltime" to "end.of.match"
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-was-bos-041616.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-was-bos-041616.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16805" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16805" uniqueCount="211">
   <si>
     <t>event</t>
   </si>
@@ -656,6 +656,9 @@
   <si>
     <t>Farquharson</t>
   </si>
+  <si>
+    <t>end.of.match</t>
+  </si>
 </sst>
 </file>
 
@@ -1264,7 +1267,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1274,9 +1277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A761" workbookViewId="0">
-      <pane xSplit="9" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M784" sqref="M784"/>
+    <sheetView tabSelected="1" topLeftCell="A1368" workbookViewId="0">
+      <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1399" sqref="F1399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -72486,7 +72489,7 @@
         <v>20</v>
       </c>
       <c r="F1399" s="23" t="s">
-        <v>136</v>
+        <v>210</v>
       </c>
       <c r="G1399" s="15" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Cleaned up disciplinary actions on all 2016 WAS home games
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-was-bos-041616.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-was-bos-041616.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/wosostats/source/excel/nwsl-2016/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1282,9 +1282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A764" workbookViewId="0">
-      <pane xSplit="9" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U783" sqref="U783"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>